<commit_message>
checking and add methods report
</commit_message>
<xml_diff>
--- a/vignettes/inst/Glossary.xlsx
+++ b/vignettes/inst/Glossary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncangillespie/Documents/qalyr/vignettes/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BD8BD0-364C-0645-B562-C2D7A235D5C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B65BC2-44D8-B246-8DE7-C02337E74E69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="480" windowWidth="19480" windowHeight="21000" xr2:uid="{45FF5812-CBE5-5C40-AB24-C165E3B43128}"/>
+    <workbookView xWindow="1940" yWindow="460" windowWidth="19480" windowHeight="21000" xr2:uid="{45FF5812-CBE5-5C40-AB24-C165E3B43128}"/>
   </bookViews>
   <sheets>
     <sheet name="glossary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Term</t>
   </si>
@@ -52,6 +52,48 @@
   </si>
   <si>
     <t>Utility scores usually range between 1 (perfect health) and 0 (a state equivalent to death), though it is possible for some extreme conditions to be valued as worse than death. The utility scores are an expression of societal preference for health states with several different methods available to estimate them. Also known as the Health state utility value (HSUV)</t>
+  </si>
+  <si>
+    <t>STAPM</t>
+  </si>
+  <si>
+    <t>The Sheffield Tobacco and Alcohol Policy Modelling - used to estimate the health and economic outcomes of changes to tobacco and/or alcohol consumption</t>
+  </si>
+  <si>
+    <t>HODaR</t>
+  </si>
+  <si>
+    <t>Health Outcomes Data Repository - the data source that we use to calculate disease specific utility scores</t>
+  </si>
+  <si>
+    <t>QoL</t>
+  </si>
+  <si>
+    <t>Quality of life</t>
+  </si>
+  <si>
+    <t>SAPM</t>
+  </si>
+  <si>
+    <t>The Sheffield Alcohol Policy Model</t>
+  </si>
+  <si>
+    <t>Finished consultant episode (FCE) or just 'episode'</t>
+  </si>
+  <si>
+    <t>The time a patient spends in the continuous care of one consultant using hospital site bed of one health care provider</t>
+  </si>
+  <si>
+    <t>ICD-10 code</t>
+  </si>
+  <si>
+    <t>International Statistical Classification of Diseases and Related Health Problems 10th Revision https://icd.who.int/</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>Adjustment factor applied to the mean general population utility score to produce estimates of utility scores for each condition that vary by age and sex</t>
   </si>
 </sst>
 </file>
@@ -406,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D218633-026C-C040-A0B4-8E1AF859BAB2}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,6 +485,62 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>